<commit_message>
fix bug edit nim
</commit_message>
<xml_diff>
--- a/upload/temp/soal-twk.xlsx
+++ b/upload/temp/soal-twk.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\cat_dua\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\soal tes p3k\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F2A877-1247-4263-BEFD-198D0F257E9F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="11310" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="190">
   <si>
     <t>bobot</t>
   </si>
@@ -238,13 +239,364 @@
   </si>
   <si>
     <t>Mau menyumbangkan harta untuk masyaraka</t>
+  </si>
+  <si>
+    <t>Perundingan antara Indonesia dan Belanda yang dilakukan pada tanggal 10 November 1945. Dalam perundingan ini, Indonesia diwakili oleh Perdana menteri Sutan Syahrir, sedangkan Belanda diwakili oleh Prof. Schermerhorn, perundingan ini adalah…</t>
+  </si>
+  <si>
+    <t>Renville</t>
+  </si>
+  <si>
+    <t>Linggarjati</t>
+  </si>
+  <si>
+    <t>Roem Royen</t>
+  </si>
+  <si>
+    <t>Giyanti</t>
+  </si>
+  <si>
+    <t>Bongaya</t>
+  </si>
+  <si>
+    <t>Perjuangan bangsa Indonesia melawan penjajah pada masa sebelum dan sesudah tahun 1928 memiliki perbedaan, pperbedaan tersebut ialah…</t>
+  </si>
+  <si>
+    <t>Sebelum 1928 menggunakan senjata, sesudah 1928 menggunakan diplomasi</t>
+  </si>
+  <si>
+    <t>sebelum 1928 bersifat kedaerahan, sesudah 1928 bersifat nasional</t>
+  </si>
+  <si>
+    <t>sebelum 1928 tidak terdapat tokoh terpelajar, sesudah 1928 terdapat tokoh terpelajar</t>
+  </si>
+  <si>
+    <t>sebelum 1928 melawan Belanda, sesudah 1928 melawan Jepang</t>
+  </si>
+  <si>
+    <t>sebelum 1928 melalui organisasi kepemudaan,  sesudah 1928 melalui partai politik</t>
+  </si>
+  <si>
+    <t>Lambang negara burung Garuda yang bertuliskan semboyan Bhineka Tunggal Ika dirancang oleh…</t>
+  </si>
+  <si>
+    <t>Ahmad Subarjo</t>
+  </si>
+  <si>
+    <t>Moh Yamin</t>
+  </si>
+  <si>
+    <t>H. Agus Salim</t>
+  </si>
+  <si>
+    <t>A. A Maramis</t>
+  </si>
+  <si>
+    <t>Sultan Hamid H</t>
+  </si>
+  <si>
+    <t>Didalam wawasan Nusantara, wawasan mengandung arti….</t>
+  </si>
+  <si>
+    <t>Pandangan, tinjauan, dan penglihatan</t>
+  </si>
+  <si>
+    <t>Pengetahuan dan pengertian</t>
+  </si>
+  <si>
+    <t>Ruang lingkup kajian</t>
+  </si>
+  <si>
+    <t>Mawas diri</t>
+  </si>
+  <si>
+    <t>Teliti dan cermat serta bijaksana</t>
+  </si>
+  <si>
+    <t>Salah satu fungsi yang dijalankan oleh LSM ataupun kelompok-kelompok kepentingan adalah Menyusun dan mengungkapkan tuntutan politik terhadap Negara, Fungsi ini disebut…</t>
+  </si>
+  <si>
+    <t>Fungsi perumusan kepentingan</t>
+  </si>
+  <si>
+    <t>Fungsi pembuatan kebijakan umum</t>
+  </si>
+  <si>
+    <t>Fungsi penerapan kebijakan</t>
+  </si>
+  <si>
+    <t>Fungsi pengawasan pelaksanaan kebijakan</t>
+  </si>
+  <si>
+    <t>Fungsi pemaduan kepentingan</t>
+  </si>
+  <si>
+    <t>Toleransi kehidupan antar-umat beragama berarti…</t>
+  </si>
+  <si>
+    <t>Persebaran agama dapat dilakukan kepda siapa saja dan dimana saja</t>
+  </si>
+  <si>
+    <t>Setiap agama memiliki tujuan dan cara ibadah yang sama kepada Tuhan</t>
+  </si>
+  <si>
+    <t>Tersedianya tempat beribadah bagi semua umat beragama dan berdekatan</t>
+  </si>
+  <si>
+    <t>Setiap orang boleh berpindah dan berganti agama setiap sata, bila dikehendaki</t>
+  </si>
+  <si>
+    <t>Menghargai aktifitas inter dan antar-umat beragama serta pemetintah</t>
+  </si>
+  <si>
+    <t>Toleransi beragama dalam kehidupan berbangsa dan bernegara ditunagkan dalam Mewujudkan nasionalisme yang tinggi dari rakyat Indonesia, yang lebih mengutamakan kepentingan nasional daripada kepentingan golongan merupakan….</t>
+  </si>
+  <si>
+    <t>Tujuan ketahanan nasional</t>
+  </si>
+  <si>
+    <t>Pengertian ketahanan nasional</t>
+  </si>
+  <si>
+    <t>Tujuan pembangunan nasional</t>
+  </si>
+  <si>
+    <t>Pengawasan wawasan nusantara</t>
+  </si>
+  <si>
+    <t>Tujuan wawasan nusantara</t>
+  </si>
+  <si>
+    <t>Munculnya kesadaran berbangsa di kalangan penduduk Indonesia didorong mula-mula oleh…</t>
+  </si>
+  <si>
+    <t>Kaum Intelektual belanda</t>
+  </si>
+  <si>
+    <t>Kaum Intelektual Indonesia</t>
+  </si>
+  <si>
+    <t>Para Ulama</t>
+  </si>
+  <si>
+    <t>Para Musyafir</t>
+  </si>
+  <si>
+    <t>Para pedagang</t>
+  </si>
+  <si>
+    <t>Jika anda menjadi anggota yang melanggar pakta integritas, maka ketika mendapat teguran biasanya Anda….</t>
+  </si>
+  <si>
+    <t>Memberi alasan yang dapat diterima mengapa saya melanggar pakta integritas</t>
+  </si>
+  <si>
+    <t>Saya akan menerima teguran tersebut karena memang salah meskipun menghadapi konsekuensinya juga akan disalahkan anggota yang lain</t>
+  </si>
+  <si>
+    <t>Menemui anggota sebelum mendapat teguran</t>
+  </si>
+  <si>
+    <t>Menunggu dipanggil dan mempersiapkan jawaban-jawaban yang akan saya berikan</t>
+  </si>
+  <si>
+    <t>Pasrah akan nasib yang saya terima</t>
+  </si>
+  <si>
+    <t>Kemajemukan sosial budaya dalam masyarakat Indonesia mempunyai pengaruh positif terhadap usaha untuk meningkatkan ketahanan nasional dalam bentuk potensi…</t>
+  </si>
+  <si>
+    <t>Akulturasi budaya</t>
+  </si>
+  <si>
+    <t>Integritas sosial</t>
+  </si>
+  <si>
+    <t>Sumber daya alam</t>
+  </si>
+  <si>
+    <t>Sumber daya manusia</t>
+  </si>
+  <si>
+    <t>Keberhasilan pembangunan</t>
+  </si>
+  <si>
+    <t>Pancasila digunakan sebagai sumber nilai-nilai yang menjadi dasar timbulnya peraturan-peraturan hukum di negara kita merupakan fungsi dan peranan Pancasila sebagai…</t>
+  </si>
+  <si>
+    <t>Dasar negara</t>
+  </si>
+  <si>
+    <t>Pandangan hidup</t>
+  </si>
+  <si>
+    <t>Perjanjian luhur</t>
+  </si>
+  <si>
+    <t>Sumber hukum dasar nasional</t>
+  </si>
+  <si>
+    <t>Pernyataan yang termasuk kewaspadaan terhadap ancaman bidang sosial budaya yaitu…</t>
+  </si>
+  <si>
+    <t>Berlomba-lomba untuk membangun bangsa dan negara</t>
+  </si>
+  <si>
+    <t>Tidak ada perbedaan antara si kaya dan si miskin</t>
+  </si>
+  <si>
+    <t>Meningkatkan kesetiakawanan sosial dalam masyarakat</t>
+  </si>
+  <si>
+    <t>Memberikan semangat tenggang rasa dan toleransi</t>
+  </si>
+  <si>
+    <t>Berkarya untuk kepentingan bangsa dan negara</t>
+  </si>
+  <si>
+    <t>Dalam proses pengambilan keputusan, sikap Anda adalah ....</t>
+  </si>
+  <si>
+    <t>Melontarkan gagasan yang memancing keterlibatan anggota</t>
+  </si>
+  <si>
+    <t>Mengambil alih proses pengambilan keputusan</t>
+  </si>
+  <si>
+    <t>Mengusahakan agar pendapat Anda diterima</t>
+  </si>
+  <si>
+    <t>Menciptakan suasana agar orang berani mengungkapkan pendapatnya</t>
+  </si>
+  <si>
+    <t>Mempercayakan keputusan pada kelompok</t>
+  </si>
+  <si>
+    <t>Salah satu pahlawan nasional yang merupakan jurnalis dan aktivis kemerdekaan dan Wakil Presiden Indonesia ketiga adalah….</t>
+  </si>
+  <si>
+    <t>Ahmad Yusuf</t>
+  </si>
+  <si>
+    <t>Sukarni</t>
+  </si>
+  <si>
+    <t>Adam Malik</t>
+  </si>
+  <si>
+    <t>Umar Wirahadikusumah</t>
+  </si>
+  <si>
+    <t>Boediono</t>
+  </si>
+  <si>
+    <t>Sidang BPUPKI pertama dilaksanakan pada 29 Mei – 1 Juni 1945 membahas mengenai perumusan Pancasila sebagai calon dasar negara. Sidang tersebut diketuai oleh….</t>
+  </si>
+  <si>
+    <t>Soekarno</t>
+  </si>
+  <si>
+    <t>Moh. Hatta</t>
+  </si>
+  <si>
+    <t>Moh. Yamin</t>
+  </si>
+  <si>
+    <t>Soetomo</t>
+  </si>
+  <si>
+    <t>Radjiman Widyodiningrat</t>
+  </si>
+  <si>
+    <t>Pancasila dijadikan sebagai ... dalam sumber tata hukum di Indonesia</t>
+  </si>
+  <si>
+    <t>Hukum tertulis tertinggi</t>
+  </si>
+  <si>
+    <t>Setingkat dengan UUD 1945</t>
+  </si>
+  <si>
+    <t>Sumber dari segala sumber hukum</t>
+  </si>
+  <si>
+    <t>Setingkat dengan TAP MPR</t>
+  </si>
+  <si>
+    <t>Hukum tertinggi</t>
+  </si>
+  <si>
+    <t>Pancasila sebagai pegangan masyarakat dalam bersikap dan berperilaku sehari-hari merupakan….</t>
+  </si>
+  <si>
+    <t>Sumber hukum bagi bangsa dan negara</t>
+  </si>
+  <si>
+    <t>Pandangan hidup bangsa</t>
+  </si>
+  <si>
+    <t>Cita-cita dan tujuan bangsa</t>
+  </si>
+  <si>
+    <t>Nilai-nilai luhur bangsa</t>
+  </si>
+  <si>
+    <t>Fungsi DPR diatur dalam UUD 1945 pada ...</t>
+  </si>
+  <si>
+    <t>Pasal 11 Ayat (2)</t>
+  </si>
+  <si>
+    <t>Pasal 14 Ayat (1)</t>
+  </si>
+  <si>
+    <t>Pasal 20A Ayat (1)</t>
+  </si>
+  <si>
+    <t>Pasal 20A Ayat (2)</t>
+  </si>
+  <si>
+    <t>Pasal 22E Ayat (1)</t>
+  </si>
+  <si>
+    <t>Amandemen Undang-Undang Dasar 1945 kedua kali dilakukan pada ...</t>
+  </si>
+  <si>
+    <t>18 Agustus 2000</t>
+  </si>
+  <si>
+    <t>19 Oktober 2000</t>
+  </si>
+  <si>
+    <t>16 Juli 2001</t>
+  </si>
+  <si>
+    <t>11 Agustus 2002</t>
+  </si>
+  <si>
+    <t>Lembaga tinggi negara yang anggotanya merupakan perwakilan dari setiap provinsi adalah …..</t>
+  </si>
+  <si>
+    <t>DPR</t>
+  </si>
+  <si>
+    <t>MPR</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>DPD</t>
+  </si>
+  <si>
+    <t>DPRD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,25 +606,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <b/>
       <i/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <color rgb="FF10242A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <color rgb="FF323233"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF14142B"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -301,22 +664,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,6 +819,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -446,6 +871,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -621,13 +1063,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -658,7 +1100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,63 +1126,63 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="114" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7.5</v>
+    <row r="3" spans="1:15" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>7.5</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>7.5</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -752,380 +1194,734 @@
       <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>7.5</v>
+    <row r="6" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7.5</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7.5</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7.5</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7.5</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:15" ht="63" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7.5</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>7.5</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:15" ht="63" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>5</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>5</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>5</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>5</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>5</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>5</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>5</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>5</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>5</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>5</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>5</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>5</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>5</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>5</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>5</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>5</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="G31" s="20">
+        <v>37204</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>5</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" x14ac:dyDescent="0.25"/>
+    <row r="34" x14ac:dyDescent="0.25"/>
+    <row r="35" x14ac:dyDescent="0.25"/>
+    <row r="36" x14ac:dyDescent="0.25"/>
+    <row r="37" x14ac:dyDescent="0.25"/>
+    <row r="38" x14ac:dyDescent="0.25"/>
+    <row r="39" x14ac:dyDescent="0.25"/>
+    <row r="40" x14ac:dyDescent="0.25"/>
+    <row r="41" x14ac:dyDescent="0.25"/>
+    <row r="42" x14ac:dyDescent="0.25"/>
+    <row r="43" x14ac:dyDescent="0.25"/>
+    <row r="44" x14ac:dyDescent="0.25"/>
+    <row r="45" x14ac:dyDescent="0.25"/>
+    <row r="46" x14ac:dyDescent="0.25"/>
+    <row r="47" x14ac:dyDescent="0.25"/>
+    <row r="48" x14ac:dyDescent="0.25"/>
     <row r="49" x14ac:dyDescent="0.25"/>
     <row r="50" x14ac:dyDescent="0.25"/>
     <row r="51" x14ac:dyDescent="0.25"/>
@@ -1187,11 +1983,11 @@
     <row r="107" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H107">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H102" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$K$1:$O$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>